<commit_message>
Atualizando testes da 2° Sprint
</commit_message>
<xml_diff>
--- a/docs/testcases/Testes Funcionais - Sprint 2.xlsx
+++ b/docs/testcases/Testes Funcionais - Sprint 2.xlsx
@@ -327,38 +327,38 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin"/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -427,7 +427,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -439,11 +439,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -455,11 +455,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -471,7 +471,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -479,15 +479,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -495,7 +495,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -531,7 +531,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -539,15 +539,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -636,12 +636,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="81.3979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="80.4540816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>